<commit_message>
added Organizational UnitID and other things
</commit_message>
<xml_diff>
--- a/Transformed Energy SourceData.xlsx
+++ b/Transformed Energy SourceData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Etech\RodanXD\ELTpart2\etl_pipeline_schema_mapping (1)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankun\MydjangoEnv\ELT-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04412A41-37FB-4E83-9604-84672FA5272A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D53B83-5630-45A8-985A-464FC0875446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -594,7 +594,7 @@
     <t>INV-ENERGY-2023-153</t>
   </si>
   <si>
-    <t>SAR</t>
+    <t>EUR</t>
   </si>
 </sst>
 </file>
@@ -864,7 +864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L153"/>
     </sheetView>
   </sheetViews>

</xml_diff>